<commit_message>
Personenstunden für Daniel Spaniol engetragen
</commit_message>
<xml_diff>
--- a/Unterlagen/Projektstunden.xlsx
+++ b/Unterlagen/Projektstunden.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Studium\ProjectManagement\Team-Gold\Unterlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="1068" yWindow="0" windowWidth="19380" windowHeight="8340" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Projektablaufplan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Spaniol" sheetId="5" r:id="rId6"/>
     <sheet name="Häßel" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -90,12 +90,138 @@
   </si>
   <si>
     <t>Abschlusspräsentation, Allgemeines</t>
+  </si>
+  <si>
+    <t>Coding-Guidelines erstellt</t>
+  </si>
+  <si>
+    <t>Erste Ideen für Engine</t>
+  </si>
+  <si>
+    <t>Erstes Konzept für Engine fertig</t>
+  </si>
+  <si>
+    <t>Überarbeitung Konzept für Engine</t>
+  </si>
+  <si>
+    <t>Konzept für Engine abschließen</t>
+  </si>
+  <si>
+    <t>Core-Modul der Engine angefangen</t>
+  </si>
+  <si>
+    <t>Core-Modul der Engine weiter bearbeiten</t>
+  </si>
+  <si>
+    <t>Erste Ideen für Game-Architektur</t>
+  </si>
+  <si>
+    <t>Service-Modul der Engine angefangen</t>
+  </si>
+  <si>
+    <t>Weitere Ideen für Game-Architektur</t>
+  </si>
+  <si>
+    <t>Paketstruktur für Game festgelegt</t>
+  </si>
+  <si>
+    <t>Service-Modul der Engine abgeschlossen</t>
+  </si>
+  <si>
+    <t>Core-Modul der Engine (vorerst) abgeschlossen</t>
+  </si>
+  <si>
+    <t>Architektur Game abgeschlossen</t>
+  </si>
+  <si>
+    <t>Kleine Überarbeitung des Core-Modules</t>
+  </si>
+  <si>
+    <t>Überarbeitung des Service-Modules (@Inject, …)</t>
+  </si>
+  <si>
+    <t>Behavior-Modul der Engine angefangen</t>
+  </si>
+  <si>
+    <t>Behavior-Modul der Engine weiter bearbeitet</t>
+  </si>
+  <si>
+    <t>Abschließende Gedanken zum Game (Spielstand speichern, …)</t>
+  </si>
+  <si>
+    <t>Default-Services angefangen</t>
+  </si>
+  <si>
+    <t>Core-Modul erweitert &amp; Behavior-Modul weiter bearbetet</t>
+  </si>
+  <si>
+    <t>Behavior-Modul abgeschlossen &amp; Einbindung in Scene</t>
+  </si>
+  <si>
+    <t>Game-Services angefangen</t>
+  </si>
+  <si>
+    <t>Package-Setup für Game</t>
+  </si>
+  <si>
+    <t>Default-Services weiter bearbeitet</t>
+  </si>
+  <si>
+    <t>Daten-Typ Klassen für Spielstand angelegt (Konzept hat gefehlt….)</t>
+  </si>
+  <si>
+    <t>Engine (vorerst) abgeschlossen (Behavior und Core Refactoring)</t>
+  </si>
+  <si>
+    <t>JavaDoc Core überarbeitet</t>
+  </si>
+  <si>
+    <t>JavaDoc Services &amp; Default-Services überarbeitet</t>
+  </si>
+  <si>
+    <t>JavaDoc Engine fertig</t>
+  </si>
+  <si>
+    <t>Tutorial für Engine geschrieben (Spieleentwicklung.html)</t>
+  </si>
+  <si>
+    <t>Implementierungsklassen zu inneren Klassen gemacht</t>
+  </si>
+  <si>
+    <t>Game-Services für Gameplay geschrieben</t>
+  </si>
+  <si>
+    <t>JavaDoc für Game-Services geschrieben</t>
+  </si>
+  <si>
+    <t>Alle Scene-Klassen angelegt &amp; Ids vergeben</t>
+  </si>
+  <si>
+    <t>Default-Components geschrieben</t>
+  </si>
+  <si>
+    <t>Default-Prefabs geschrieben</t>
+  </si>
+  <si>
+    <t>Manche Default Components und Prefabs in die Engine</t>
+  </si>
+  <si>
+    <t>JavaDoc Default Components überarbeitet</t>
+  </si>
+  <si>
+    <t>Kleine Änderungen and Default Components und Prefabs</t>
+  </si>
+  <si>
+    <t>Überarbeitung der Game-Spezifischen Post-Game-Screens</t>
+  </si>
+  <si>
+    <t>Abschließende Überarbeitungen an der CodeBase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -227,6 +353,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2770,111 +2899,160 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="7648575"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Textfeld 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="7648575"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Textfeld 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="419100" y="7648575"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>40</xdr:row>
+        <xdr:cNvPr id="6" name="Textfeld 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="7915275"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Textfeld 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="419100" y="7648575"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Textfeld 5"/>
+        <xdr:cNvPr id="7" name="Textfeld 6"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2917,56 +3095,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Textfeld 6"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="419100" y="7915275"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -3019,8 +3148,8 @@
       <xdr:rowOff>19054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3741419</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>110917</xdr:rowOff>
     </xdr:to>
@@ -3048,6 +3177,104 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Textfeld 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="7620000"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Textfeld 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="7620000"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3241,7 +3468,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3316,6 +3543,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3351,6 +3595,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3509,7 +3770,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3519,25 +3780,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3548,8 +3809,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42473</v>
       </c>
@@ -3560,7 +3821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>42474</v>
       </c>
@@ -3571,7 +3832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>42478</v>
       </c>
@@ -3582,7 +3843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>42485</v>
       </c>
@@ -3593,7 +3854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42487</v>
       </c>
@@ -3604,7 +3865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>42488</v>
       </c>
@@ -3615,7 +3876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>42492</v>
       </c>
@@ -3626,7 +3887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>42469</v>
       </c>
@@ -3637,7 +3898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>42471</v>
       </c>
@@ -3648,7 +3909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>42508</v>
       </c>
@@ -3659,7 +3920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>42529</v>
       </c>
@@ -3670,7 +3931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>42534</v>
       </c>
@@ -3681,7 +3942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>42536</v>
       </c>
@@ -3692,133 +3953,133 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>3</v>
       </c>
@@ -3845,21 +4106,21 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3870,198 +4131,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>3</v>
       </c>
@@ -4087,21 +4348,21 @@
       <selection activeCell="C8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4112,198 +4373,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>3</v>
       </c>
@@ -4329,21 +4590,21 @@
       <selection activeCell="B19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4354,198 +4615,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>3</v>
       </c>
@@ -4565,27 +4826,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4596,204 +4857,515 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A43" s="9" t="s">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>42499</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>42499</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>42501</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>42501</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>42503</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>42504</v>
+      </c>
+      <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="B43" s="7">
-        <f>SUM(B4:B41)</f>
-        <v>0</v>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>42505</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>42506</v>
+      </c>
+      <c r="B11" s="5">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>42507</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>42508</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>42509</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>42509</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>42510</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>42511</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>42511</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>42512</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>42513</v>
+      </c>
+      <c r="B20" s="5">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>42514</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>42515</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>42516</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>42516</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>42516</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>42517</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>42518</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>42519</v>
+      </c>
+      <c r="B28" s="5">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>42520</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>42521</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>42521</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>42156</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>42157</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>42524</v>
+      </c>
+      <c r="B34" s="5">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>42525</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>42526</v>
+      </c>
+      <c r="B36" s="5">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>42526</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>42527</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>42528</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>42529</v>
+      </c>
+      <c r="B40" s="5">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>42530</v>
+      </c>
+      <c r="B41" s="5">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>42531</v>
+      </c>
+      <c r="B42" s="5">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42532</v>
+      </c>
+      <c r="B43" s="5">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>42533</v>
+      </c>
+      <c r="B44" s="5">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>42534</v>
+      </c>
+      <c r="B45" s="5">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>42534</v>
+      </c>
+      <c r="B46" s="5">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>42535</v>
+      </c>
+      <c r="B47" s="5">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>42536</v>
+      </c>
+      <c r="B48" s="5">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="15"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A51" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7">
+        <f>SUM(B4:B48)</f>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4813,21 +5385,21 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4838,198 +5410,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>